<commit_message>
resultats adv model2 + rapport
</commit_message>
<xml_diff>
--- a/Securite/Model19/adversarial/analyse courbe_model19.xlsx
+++ b/Securite/Model19/adversarial/analyse courbe_model19.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0216e4c439e2ba0d/Documents/Hugo/ISMIN/Cours/S9/E_IA/Projet/Github/ES_IA_Embedded_Project/Securite/Model19/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0216e4c439e2ba0d/Documents/Hugo/ISMIN/Cours/S9/E_IA/Projet/Github/ES_IA_Embedded_Project/Securite/Model19/adversarial/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="8_{868BEB3A-3412-4929-86D1-746D778D1B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BEED6375-9513-4FBF-90A0-15594ED92B00}"/>
+  <xr:revisionPtr revIDLastSave="66" documentId="8_{868BEB3A-3412-4929-86D1-746D778D1B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B5F0118-258F-4887-9920-58743E1A692F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4133799A-7748-4670-AD98-3E73C3625772}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -510,7 +509,377 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{50F5F5E9-07EF-4B93-A6E9-2B96FBDCD9C8}" type="CELLRANGE">
+                    <a:fld id="{53E3BA2D-C8C5-4ACE-894B-C6DB6C9DC485}" type="CELLRANGE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[PLAGECELL]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>; </a:t>
+                    </a:r>
+                    <a:fld id="{AE64A270-5FAA-4B30-9018-D418254AF4E6}" type="XVALUE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[VALEUR X]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US" baseline="0"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-9DC8-4F54-BD1A-1E4C4FBA03CD}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.5804493017607778E-2"/>
+                  <c:y val="4.5662100456621002E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{A41C72C6-9BF0-40C8-9171-FC04FF622651}" type="CELLRANGE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[PLAGECELL]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>; </a:t>
+                    </a:r>
+                    <a:fld id="{33BB3B85-4D4D-48D1-851A-478A63583B64}" type="XVALUE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[VALEUR X]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US" baseline="0"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-9DC8-4F54-BD1A-1E4C4FBA03CD}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.0358227079538623E-3"/>
+                  <c:y val="-2.7397260273972601E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{19C79080-330D-4AC2-9ED1-9A8111D0E715}" type="CELLRANGE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[PLAGECELL]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>; </a:t>
+                    </a:r>
+                    <a:fld id="{5B4ECAF2-010B-4D28-B803-5D096855758F}" type="XVALUE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[VALEUR X]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US" baseline="0"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-9DC8-4F54-BD1A-1E4C4FBA03CD}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.0716454159077107E-3"/>
+                  <c:y val="-2.4353120243531201E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{B5EDF2AB-C3A2-4666-A61E-4BF2C4A3DC98}" type="CELLRANGE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[PLAGECELL]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>; </a:t>
+                    </a:r>
+                    <a:fld id="{1CA0FDE0-6CD3-41F5-B834-1FFDECA6C858}" type="XVALUE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[VALEUR X]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US" baseline="0"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-9DC8-4F54-BD1A-1E4C4FBA03CD}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.4286581663630843E-2"/>
+                  <c:y val="4.5662100456621113E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{2C93E539-E16D-4B71-9B5B-035AA2467911}" type="CELLRANGE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[PLAGECELL]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>; </a:t>
+                    </a:r>
+                    <a:fld id="{34EC72B5-8BDD-4599-A159-4D8E6774E3AC}" type="XVALUE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[VALEUR X]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US" baseline="0"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-9DC8-4F54-BD1A-1E4C4FBA03CD}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="2.7397260273972601E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{D2928755-D07B-4348-99EB-73E3D8976D3F}" type="CELLRANGE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[PLAGECELL]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>; </a:t>
+                    </a:r>
+                    <a:fld id="{E57A129A-98AC-430A-9723-320CDD374D34}" type="XVALUE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[VALEUR X]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US" baseline="0"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-9DC8-4F54-BD1A-1E4C4FBA03CD}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-9.1074681238616784E-3"/>
+                  <c:y val="3.6529680365296913E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{C6966D1F-B8A3-47A8-ACDC-DDE8FFA1E143}" type="CELLRANGE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[PLAGECELL]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>; </a:t>
+                    </a:r>
+                    <a:fld id="{46142370-439E-409A-B46D-4F4758E530CE}" type="XVALUE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[VALEUR X]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US" baseline="0"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-9DC8-4F54-BD1A-1E4C4FBA03CD}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-2.7397260273972601E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{93EDD4CA-F4C2-4BB5-A7E5-D70270A3AC26}" type="CELLRANGE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[PLAGECELL]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>; </a:t>
+                    </a:r>
+                    <a:fld id="{15D77FEA-D6A5-4C6D-A6A9-2F79444577E0}" type="XVALUE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[VALEUR X]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US" baseline="0"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-9DC8-4F54-BD1A-1E4C4FBA03CD}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{9192BA10-6948-4573-9F12-E37ED90318DD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -519,377 +888,7 @@
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>; </a:t>
                     </a:r>
-                    <a:fld id="{F4D51B30-1040-4AC4-82E7-7CAE56ACDE72}" type="XVALUE">
-                      <a:rPr lang="en-US" baseline="0"/>
-                      <a:pPr/>
-                      <a:t>[VALEUR X]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="en-US" baseline="0"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:dlblFieldTable/>
-                  <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000000-9DC8-4F54-BD1A-1E4C4FBA03CD}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-2.5804493017607778E-2"/>
-                  <c:y val="4.5662100456621002E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{9F18BA5E-933E-4D58-A490-98245D6D1958}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
-                      <a:pPr/>
-                      <a:t>[PLAGECELL]</a:t>
-                    </a:fld>
-                    <a:r>
-                      <a:rPr lang="en-US" baseline="0"/>
-                      <a:t>; </a:t>
-                    </a:r>
-                    <a:fld id="{527B6193-F8FC-4636-ABCC-74859406DDAC}" type="XVALUE">
-                      <a:rPr lang="en-US" baseline="0"/>
-                      <a:pPr/>
-                      <a:t>[VALEUR X]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="en-US" baseline="0"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:dlblFieldTable/>
-                  <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000001-9DC8-4F54-BD1A-1E4C4FBA03CD}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-3.0358227079538623E-3"/>
-                  <c:y val="-2.7397260273972601E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{60773052-5D60-45D6-B0AE-E3B38972326C}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
-                      <a:pPr/>
-                      <a:t>[PLAGECELL]</a:t>
-                    </a:fld>
-                    <a:r>
-                      <a:rPr lang="en-US" baseline="0"/>
-                      <a:t>; </a:t>
-                    </a:r>
-                    <a:fld id="{0E613355-5794-49BA-8966-4A05764F9537}" type="XVALUE">
-                      <a:rPr lang="en-US" baseline="0"/>
-                      <a:pPr/>
-                      <a:t>[VALEUR X]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="en-US" baseline="0"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:dlblFieldTable/>
-                  <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000002-9DC8-4F54-BD1A-1E4C4FBA03CD}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-6.0716454159077107E-3"/>
-                  <c:y val="-2.4353120243531201E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{ACF95A05-9F47-4C9D-AD8E-7400A715D2A8}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
-                      <a:pPr/>
-                      <a:t>[PLAGECELL]</a:t>
-                    </a:fld>
-                    <a:r>
-                      <a:rPr lang="en-US" baseline="0"/>
-                      <a:t>; </a:t>
-                    </a:r>
-                    <a:fld id="{3C1DBD50-0063-4601-970F-88EFD983B28D}" type="XVALUE">
-                      <a:rPr lang="en-US" baseline="0"/>
-                      <a:pPr/>
-                      <a:t>[VALEUR X]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="en-US" baseline="0"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:dlblFieldTable/>
-                  <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-9DC8-4F54-BD1A-1E4C4FBA03CD}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-2.4286581663630843E-2"/>
-                  <c:y val="4.5662100456621113E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{C9ADB77F-586E-42C7-B877-984A1BFAB4CE}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
-                      <a:pPr/>
-                      <a:t>[PLAGECELL]</a:t>
-                    </a:fld>
-                    <a:r>
-                      <a:rPr lang="en-US" baseline="0"/>
-                      <a:t>; </a:t>
-                    </a:r>
-                    <a:fld id="{62AF0D60-F964-42AA-B175-0BC9EAF459A5}" type="XVALUE">
-                      <a:rPr lang="en-US" baseline="0"/>
-                      <a:pPr/>
-                      <a:t>[VALEUR X]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="en-US" baseline="0"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:dlblFieldTable/>
-                  <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000004-9DC8-4F54-BD1A-1E4C4FBA03CD}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0"/>
-                  <c:y val="2.7397260273972601E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{9A20CE2D-C5F9-426B-8B0E-BD3584E1958B}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
-                      <a:pPr/>
-                      <a:t>[PLAGECELL]</a:t>
-                    </a:fld>
-                    <a:r>
-                      <a:rPr lang="en-US" baseline="0"/>
-                      <a:t>; </a:t>
-                    </a:r>
-                    <a:fld id="{FDD08C24-1965-46DD-AAC5-DEFC880C144B}" type="XVALUE">
-                      <a:rPr lang="en-US" baseline="0"/>
-                      <a:pPr/>
-                      <a:t>[VALEUR X]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="en-US" baseline="0"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:dlblFieldTable/>
-                  <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000005-9DC8-4F54-BD1A-1E4C4FBA03CD}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="6"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-9.1074681238616784E-3"/>
-                  <c:y val="3.6529680365296913E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{165B26DE-D667-488B-8767-0AF8FD42DF19}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
-                      <a:pPr/>
-                      <a:t>[PLAGECELL]</a:t>
-                    </a:fld>
-                    <a:r>
-                      <a:rPr lang="en-US" baseline="0"/>
-                      <a:t>; </a:t>
-                    </a:r>
-                    <a:fld id="{2055A315-4C5B-483B-A555-8F053F88E2C6}" type="XVALUE">
-                      <a:rPr lang="en-US" baseline="0"/>
-                      <a:pPr/>
-                      <a:t>[VALEUR X]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="en-US" baseline="0"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:dlblFieldTable/>
-                  <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000006-9DC8-4F54-BD1A-1E4C4FBA03CD}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="7"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0"/>
-                  <c:y val="-2.7397260273972601E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{EC5B3AC6-2DC8-4173-874A-43AC744F52DA}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
-                      <a:pPr/>
-                      <a:t>[PLAGECELL]</a:t>
-                    </a:fld>
-                    <a:r>
-                      <a:rPr lang="en-US" baseline="0"/>
-                      <a:t>; </a:t>
-                    </a:r>
-                    <a:fld id="{143B03E9-5E59-477F-812D-7B14074B4D11}" type="XVALUE">
-                      <a:rPr lang="en-US" baseline="0"/>
-                      <a:pPr/>
-                      <a:t>[VALEUR X]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="en-US" baseline="0"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:dlblFieldTable/>
-                  <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000007-9DC8-4F54-BD1A-1E4C4FBA03CD}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="8"/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{FB9EA0DB-CA2F-4AD9-830A-D7CBA0985E19}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
-                      <a:pPr/>
-                      <a:t>[PLAGECELL]</a:t>
-                    </a:fld>
-                    <a:r>
-                      <a:rPr lang="en-US" baseline="0"/>
-                      <a:t>; </a:t>
-                    </a:r>
-                    <a:fld id="{B7DE9F08-4C18-461B-8012-D2FBC83A7587}" type="XVALUE">
+                    <a:fld id="{F2E6BFE9-452C-4769-ABD7-BC9E89C4B699}" type="XVALUE">
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
                       <a:t>[VALEUR X]</a:t>
@@ -4127,16 +4126,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>87630</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>777240</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>64770</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>411480</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>426720</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>

</xml_diff>